<commit_message>
add intensities, more energies to data
</commit_message>
<xml_diff>
--- a/data-raw/Salem et al. 1974 Table I.xlsx
+++ b/data-raw/Salem et al. 1974 Table I.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/dewey/d/rdevel/xrf/data-raw/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BE5D96C5-1A35-0F40-ADB3-3B626751D405}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3B2A1CFF-199D-EA4F-88C3-128D914ED130}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="19900" yWindow="880" windowWidth="12240" windowHeight="17440" xr2:uid="{875243E4-C799-B34A-A4E1-33F7F4DC4A89}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="54" uniqueCount="53">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="54" uniqueCount="54">
   <si>
     <t>Element</t>
   </si>
@@ -184,6 +184,9 @@
   </si>
   <si>
     <t>Er</t>
+  </si>
+  <si>
+    <t>S</t>
   </si>
 </sst>
 </file>
@@ -539,8 +542,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{690527C7-E8CB-A544-9304-D0A08F110D40}">
   <dimension ref="A1:I46"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="I28" sqref="I28"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A5" sqref="A5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -592,7 +595,7 @@
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>10</v>
+        <v>53</v>
       </c>
       <c r="I4">
         <v>5.8999999999999997E-2</v>

</xml_diff>